<commit_message>
Loads, Yolo, 5_wy2017-18: pTHg, fTHg, wwTHg, SSC: Replaced pTHg rloadest folder (made edits to script, made edits to plot headers to include the year "5_..."- cosmetic changes), added folders for fTHg, wwTHg, and SSC; updated Model Results for pTHg, added new files for fTHg, wwTHg, and SSC; updated the Yolo Q and WQ file; Added fTHg, wwTHg, and SSC PDFs for Sigma Plot and added plots to the Power Point.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/5_wy2017-2018/5_pTHg Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/5_wy2017-2018/5_pTHg Model Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\5_wy2017-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C629777A-5CE5-40B3-A795-082B7D7332A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DD74C4-2818-459A-A636-255C2D758FA3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pTHg wy2017-18 Model Results" sheetId="2" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="310">
   <si>
     <t>Model #</t>
   </si>
@@ -1000,6 +1000,9 @@
   </si>
   <si>
     <t>13.70, 15.86</t>
+  </si>
+  <si>
+    <t>13.94, 12.45</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1379,6 +1382,9 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1403,7 +1409,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2017,7 +2026,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
+      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2038,24 +2047,24 @@
       <c r="A1" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51" t="s">
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="51"/>
+      <c r="M1" s="52"/>
       <c r="N1" s="24"/>
       <c r="Q1" s="24"/>
     </row>
@@ -2190,18 +2199,18 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="46"/>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="55"/>
       <c r="L6" s="46"/>
       <c r="M6" s="46"/>
       <c r="N6" s="46"/>
@@ -2222,22 +2231,22 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" s="46"/>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="56" t="s">
         <v>306</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="58" t="s">
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="58"/>
+      <c r="M7" s="59"/>
       <c r="N7" s="46"/>
       <c r="O7" s="46"/>
       <c r="Q7" s="46"/>
@@ -2351,7 +2360,9 @@
       <c r="N9" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="O9" s="38"/>
+      <c r="O9" s="38" t="s">
+        <v>309</v>
+      </c>
       <c r="P9" s="38"/>
       <c r="Q9" s="7" t="s">
         <v>10</v>
@@ -2364,49 +2375,49 @@
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A10" s="46">
+      <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="11">
         <v>0</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="60">
         <v>9.5399999999999999E-2</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="47">
+      <c r="I10" s="11">
         <v>98.42</v>
       </c>
-      <c r="J10" s="47">
+      <c r="J10" s="11">
         <v>2.7799999999999998E-2</v>
       </c>
-      <c r="K10" s="47">
+      <c r="K10" s="11">
         <v>0.16</v>
       </c>
-      <c r="L10" s="47">
+      <c r="L10" s="11">
         <v>5.5739999999999998</v>
       </c>
       <c r="M10" s="47">
         <v>0.96030000000000004</v>
       </c>
-      <c r="N10" s="59" t="s">
+      <c r="N10" s="51" t="s">
         <v>307</v>
       </c>
-      <c r="O10" s="59" t="s">
+      <c r="O10" s="51" t="s">
         <v>308</v>
       </c>
       <c r="P10" s="38"/>
@@ -2794,37 +2805,37 @@
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="55"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B20" s="55"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="58" t="s">
+      <c r="B20" s="56"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="58"/>
+      <c r="M20" s="59"/>
       <c r="Q20" s="1"/>
     </row>
     <row r="21" spans="1:29" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -3220,37 +3231,37 @@
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B32" s="52" t="s">
+      <c r="B32" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="55"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="Q32" s="1"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B33" s="55"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="57"/>
-      <c r="L33" s="58" t="s">
+      <c r="B33" s="56"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="57"/>
+      <c r="J33" s="57"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="M33" s="58"/>
+      <c r="M33" s="59"/>
       <c r="Q33" s="1"/>
     </row>
     <row r="34" spans="1:30" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -3646,37 +3657,37 @@
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B45" s="52" t="s">
+      <c r="B45" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="54"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="54"/>
+      <c r="K45" s="55"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="Q45" s="1"/>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B46" s="55"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="58" t="s">
+      <c r="B46" s="56"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="M46" s="58"/>
+      <c r="M46" s="59"/>
       <c r="Q46" s="1"/>
     </row>
     <row r="47" spans="1:30" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -4073,37 +4084,37 @@
       <c r="AA57" s="9"/>
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B59" s="52" t="s">
+      <c r="B59" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="53"/>
-      <c r="G59" s="53"/>
-      <c r="H59" s="53"/>
-      <c r="I59" s="53"/>
-      <c r="J59" s="53"/>
-      <c r="K59" s="54"/>
-      <c r="L59" s="58"/>
-      <c r="M59" s="58"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="54"/>
+      <c r="F59" s="54"/>
+      <c r="G59" s="54"/>
+      <c r="H59" s="54"/>
+      <c r="I59" s="54"/>
+      <c r="J59" s="54"/>
+      <c r="K59" s="55"/>
+      <c r="L59" s="59"/>
+      <c r="M59" s="59"/>
       <c r="Q59" s="1"/>
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B60" s="55"/>
-      <c r="C60" s="56"/>
-      <c r="D60" s="56"/>
-      <c r="E60" s="56"/>
-      <c r="F60" s="56"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="56"/>
-      <c r="I60" s="56"/>
-      <c r="J60" s="56"/>
-      <c r="K60" s="57"/>
-      <c r="L60" s="58" t="s">
+      <c r="B60" s="56"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="57"/>
+      <c r="F60" s="57"/>
+      <c r="G60" s="57"/>
+      <c r="H60" s="57"/>
+      <c r="I60" s="57"/>
+      <c r="J60" s="57"/>
+      <c r="K60" s="58"/>
+      <c r="L60" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="M60" s="58"/>
+      <c r="M60" s="59"/>
       <c r="Q60" s="1"/>
     </row>
     <row r="61" spans="1:29" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">

</xml_diff>